<commit_message>
Refactor: Updated screenshot saving path to root Screenshots folder
</commit_message>
<xml_diff>
--- a/Excel_Files/LoginData.xlsx
+++ b/Excel_Files/LoginData.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanav\OneDrive\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EA9DD4-5222-46AE-9F08-F62AA34564BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{655BFE61-9898-424D-B6FB-A31C6F7CCA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B32FC998-9215-4351-A9D5-4469C0BCB569}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,16 +52,16 @@
     <t>kanav123</t>
   </si>
   <si>
-    <t>Student123</t>
-  </si>
-  <si>
-    <t>student</t>
-  </si>
-  <si>
-    <t>Karan</t>
-  </si>
-  <si>
-    <t>Karan12</t>
+    <t>shardul</t>
+  </si>
+  <si>
+    <t>shardul123</t>
+  </si>
+  <si>
+    <t>kiran</t>
+  </si>
+  <si>
+    <t>kiran12</t>
   </si>
 </sst>
 </file>
@@ -440,7 +436,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,10 +471,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>